<commit_message>
Fix pandas API compatibility issue in nz_util.py and add notebook format fixes
Co-authored-by: Diego Diaz <diegodiaz@uchicago.edu>
</commit_message>
<xml_diff>
--- a/article_assets/nz_outcome_extension_tables.xlsx
+++ b/article_assets/nz_outcome_extension_tables.xlsx
@@ -37,16 +37,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -62,7 +54,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -70,30 +62,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,411 +369,411 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>2000</v>
       </c>
       <c r="B2">
         <v>26604</v>
       </c>
       <c r="C2">
-        <v>26563.74324728095</v>
+        <v>26556.58015712952</v>
       </c>
       <c r="D2">
-        <v>40.25675271905129</v>
+        <v>47.41984287047671</v>
       </c>
       <c r="E2">
-        <v>0.1515477406339257</v>
+        <v>0.1785615564575852</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2001</v>
       </c>
       <c r="B3">
         <v>27799</v>
       </c>
       <c r="C3">
-        <v>28349.37859189246</v>
+        <v>28347.25180397787</v>
       </c>
       <c r="D3">
-        <v>-550.3785918924623</v>
+        <v>-548.2518039778697</v>
       </c>
       <c r="E3">
-        <v>-1.94141324864829</v>
+        <v>-1.934056280901754</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2002</v>
       </c>
       <c r="B4">
         <v>29500</v>
       </c>
       <c r="C4">
-        <v>30015.0270320791</v>
+        <v>30011.87409579987</v>
       </c>
       <c r="D4">
-        <v>-515.0270320791024</v>
+        <v>-511.8740957998707</v>
       </c>
       <c r="E4">
-        <v>-1.715897278815234</v>
+        <v>-1.705571915189085</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>2003</v>
       </c>
       <c r="B5">
         <v>30895</v>
       </c>
       <c r="C5">
-        <v>30789.21721387009</v>
+        <v>30785.90574021574</v>
       </c>
       <c r="D5">
-        <v>105.7827861299083</v>
+        <v>109.0942597842622</v>
       </c>
       <c r="E5">
-        <v>0.3435708852067039</v>
+        <v>0.3543643013294621</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>2004</v>
       </c>
       <c r="B6">
         <v>32739</v>
       </c>
       <c r="C6">
-        <v>32764.30120437427</v>
+        <v>32762.96229035686</v>
       </c>
       <c r="D6">
-        <v>-25.3012043742674</v>
+        <v>-23.96229035685974</v>
       </c>
       <c r="E6">
-        <v>-0.07722186478645089</v>
+        <v>-0.07313835099676738</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>2005</v>
       </c>
       <c r="B7">
         <v>35268</v>
       </c>
       <c r="C7">
-        <v>34679.93713122193</v>
+        <v>34678.72305017555</v>
       </c>
       <c r="D7">
-        <v>588.06286877807</v>
+        <v>589.2769498244452</v>
       </c>
       <c r="E7">
-        <v>1.695686086606668</v>
+        <v>1.699246390854239</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>2006</v>
       </c>
       <c r="B8">
         <v>36686</v>
       </c>
       <c r="C8">
-        <v>36912.74152057146</v>
+        <v>36912.16168001806</v>
       </c>
       <c r="D8">
-        <v>-226.7415205714569</v>
+        <v>-226.1616800180636</v>
       </c>
       <c r="E8">
-        <v>-0.614263561120471</v>
+        <v>-0.6127023444971889</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>2007</v>
       </c>
       <c r="B9">
         <v>38512</v>
       </c>
       <c r="C9">
-        <v>38169.78156392621</v>
+        <v>38172.02127435797</v>
       </c>
       <c r="D9">
-        <v>342.2184360737883</v>
+        <v>339.9787256420313</v>
       </c>
       <c r="E9">
-        <v>0.8965690188733351</v>
+        <v>0.890648999691331</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>2008</v>
       </c>
       <c r="B10">
         <v>40998</v>
       </c>
       <c r="C10">
-        <v>40990.59648890934</v>
+        <v>40985.66687073935</v>
       </c>
       <c r="D10">
-        <v>7.403511090662505</v>
+        <v>12.33312926064536</v>
       </c>
       <c r="E10">
-        <v>0.0180614865964823</v>
+        <v>0.03009132265565326</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>2009</v>
       </c>
       <c r="B11">
         <v>41846</v>
       </c>
       <c r="C11">
-        <v>42053.88300770527</v>
+        <v>42064.27557717169</v>
       </c>
       <c r="D11">
-        <v>-207.8830077052698</v>
+        <v>-218.2755771716911</v>
       </c>
       <c r="E11">
-        <v>-0.4943253579394339</v>
+        <v>-0.5189096309794752</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>2010</v>
       </c>
       <c r="B12">
         <v>42420</v>
       </c>
       <c r="C12">
-        <v>42180.9330886756</v>
+        <v>42181.37820617731</v>
       </c>
       <c r="D12">
-        <v>239.0669113244003</v>
+        <v>238.621793822691</v>
       </c>
       <c r="E12">
-        <v>0.5667653459012338</v>
+        <v>0.5657041186666245</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>2011</v>
       </c>
       <c r="B13">
         <v>44623</v>
       </c>
       <c r="C13">
-        <v>44072.6761916567</v>
+        <v>44075.73205593701</v>
       </c>
       <c r="D13">
-        <v>550.3238083432952</v>
+        <v>547.2679440629872</v>
       </c>
       <c r="E13">
-        <v>1.248673454614212</v>
+        <v>1.241653668663843</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>2012</v>
       </c>
       <c r="B14">
         <v>47514</v>
       </c>
       <c r="C14">
-        <v>45999.89084955435</v>
+        <v>46006.20622525735</v>
       </c>
       <c r="D14">
-        <v>1514.109150445649</v>
+        <v>1507.793774742648</v>
       </c>
       <c r="E14">
-        <v>3.291549441709855</v>
+        <v>3.277370377727149</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>2013</v>
       </c>
       <c r="B15">
         <v>49482</v>
       </c>
       <c r="C15">
-        <v>46066.09592124935</v>
+        <v>46070.52879091061</v>
       </c>
       <c r="D15">
-        <v>3415.904078750646</v>
+        <v>3411.471209089388</v>
       </c>
       <c r="E15">
-        <v>7.415223735456511</v>
+        <v>7.404888328007313</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>2014</v>
       </c>
       <c r="B16">
         <v>54177</v>
       </c>
       <c r="C16">
-        <v>48432.91512258055</v>
+        <v>48437.44088493662</v>
       </c>
       <c r="D16">
-        <v>5744.084877419453</v>
+        <v>5739.559115063377</v>
       </c>
       <c r="E16">
-        <v>11.85987847909123</v>
+        <v>11.84942682809715</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>2015</v>
       </c>
       <c r="B17">
         <v>55460</v>
       </c>
       <c r="C17">
-        <v>48787.74128709688</v>
+        <v>48784.65452206451</v>
       </c>
       <c r="D17">
-        <v>6672.258712903116</v>
+        <v>6675.345477935494</v>
       </c>
       <c r="E17">
-        <v>13.67609677529335</v>
+        <v>13.68328943462405</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>2016</v>
       </c>
       <c r="B18">
         <v>55712</v>
       </c>
       <c r="C18">
-        <v>49426.25435451405</v>
+        <v>49412.78005855967</v>
       </c>
       <c r="D18">
-        <v>6285.745645485949</v>
+        <v>6299.219941440329</v>
       </c>
       <c r="E18">
-        <v>12.71742260783287</v>
+        <v>12.74815935062761</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>2017</v>
       </c>
       <c r="B19">
         <v>56067</v>
       </c>
       <c r="C19">
-        <v>51959.89779081213</v>
+        <v>51952.00189555186</v>
       </c>
       <c r="D19">
-        <v>4107.102209187869</v>
+        <v>4114.998104448139</v>
       </c>
       <c r="E19">
-        <v>7.904369299806653</v>
+        <v>7.920769083588415</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>2018</v>
       </c>
       <c r="B20">
         <v>59214</v>
       </c>
       <c r="C20">
-        <v>55757.13111129605</v>
+        <v>55755.39313506885</v>
       </c>
       <c r="D20">
-        <v>3456.868888703953</v>
+        <v>3458.606864931149</v>
       </c>
       <c r="E20">
-        <v>6.199868644252418</v>
+        <v>6.20317904772474</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>2019</v>
       </c>
       <c r="B21">
         <v>60963</v>
       </c>
       <c r="C21">
-        <v>57742.09995903676</v>
+        <v>57735.96599455603</v>
       </c>
       <c r="D21">
-        <v>3220.900040963235</v>
+        <v>3227.034005443973</v>
       </c>
       <c r="E21">
-        <v>5.57807915411493</v>
+        <v>5.589295943793948</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>2020</v>
       </c>
       <c r="B22">
         <v>63380</v>
       </c>
       <c r="C22">
-        <v>59403.40771517763</v>
+        <v>59396.35117674874</v>
       </c>
       <c r="D22">
-        <v>3976.592284822371</v>
+        <v>3983.648823251264</v>
       </c>
       <c r="E22">
-        <v>6.694215766019679</v>
+        <v>6.706891491359322</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>2021</v>
       </c>
       <c r="B23">
         <v>62198</v>
       </c>
       <c r="C23">
-        <v>60915.53127569849</v>
+        <v>60905.88655061334</v>
       </c>
       <c r="D23">
-        <v>1282.468724301507</v>
+        <v>1292.113449386663</v>
       </c>
       <c r="E23">
-        <v>2.105323055457176</v>
+        <v>2.121491899330461</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>2022</v>
       </c>
       <c r="B24">
         <v>67455</v>
       </c>
       <c r="C24">
-        <v>65359.72439147593</v>
+        <v>65343.15248542746</v>
       </c>
       <c r="D24">
-        <v>2095.275608524069</v>
+        <v>2111.847514572539</v>
       </c>
       <c r="E24">
-        <v>3.205759553045683</v>
+        <v>3.2319339276499</v>
       </c>
     </row>
   </sheetData>
@@ -816,411 +790,411 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>2000</v>
       </c>
       <c r="B2">
         <v>493500</v>
       </c>
       <c r="C2">
-        <v>484659.6700423952</v>
+        <v>484685.6265208999</v>
       </c>
       <c r="D2">
-        <v>8840.329957604816</v>
+        <v>8814.373479100119</v>
       </c>
       <c r="E2">
-        <v>1.824028386110921</v>
+        <v>1.818575380988741</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2001</v>
       </c>
       <c r="B3">
         <v>496200</v>
       </c>
       <c r="C3">
-        <v>489804.3037637259</v>
+        <v>489816.3383665308</v>
       </c>
       <c r="D3">
-        <v>6395.696236274089</v>
+        <v>6383.661633469164</v>
       </c>
       <c r="E3">
-        <v>1.30576562662448</v>
+        <v>1.303276582148686</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2002</v>
       </c>
       <c r="B4">
         <v>501700</v>
       </c>
       <c r="C4">
-        <v>498522.2208034463</v>
+        <v>498545.7708089837</v>
       </c>
       <c r="D4">
-        <v>3177.779196553689</v>
+        <v>3154.229191016289</v>
       </c>
       <c r="E4">
-        <v>0.6374398299502482</v>
+        <v>0.6326859790421977</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>2003</v>
       </c>
       <c r="B5">
         <v>511200</v>
       </c>
       <c r="C5">
-        <v>511892.7930886131</v>
+        <v>511948.5609111016</v>
       </c>
       <c r="D5">
-        <v>-692.7930886131362</v>
+        <v>-748.5609111016383</v>
       </c>
       <c r="E5">
-        <v>-0.1353394886521107</v>
+        <v>-0.1462179930283315</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>2004</v>
       </c>
       <c r="B6">
         <v>521200</v>
       </c>
       <c r="C6">
-        <v>523975.4355073093</v>
+        <v>524050.6765385518</v>
       </c>
       <c r="D6">
-        <v>-2775.435507309332</v>
+        <v>-2850.67653855175</v>
       </c>
       <c r="E6">
-        <v>-0.5296880958975061</v>
+        <v>-0.5439696323609345</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>2005</v>
       </c>
       <c r="B7">
         <v>529400</v>
       </c>
       <c r="C7">
-        <v>532716.3693643269</v>
+        <v>532793.9584914244</v>
       </c>
       <c r="D7">
-        <v>-3316.369364326936</v>
+        <v>-3393.958491424448</v>
       </c>
       <c r="E7">
-        <v>-0.622539414038328</v>
+        <v>-0.6370114445430738</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>2006</v>
       </c>
       <c r="B8">
         <v>536900</v>
       </c>
       <c r="C8">
-        <v>540691.5910779272</v>
+        <v>540777.7451329936</v>
       </c>
       <c r="D8">
-        <v>-3791.591077927151</v>
+        <v>-3877.745132993557</v>
       </c>
       <c r="E8">
-        <v>-0.7012483901161111</v>
+        <v>-0.7170681796529742</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>2007</v>
       </c>
       <c r="B9">
         <v>544800</v>
       </c>
       <c r="C9">
-        <v>548097.1862080466</v>
+        <v>548194.7219745264</v>
       </c>
       <c r="D9">
-        <v>-3297.186208046624</v>
+        <v>-3394.721974526416</v>
       </c>
       <c r="E9">
-        <v>-0.6015696287108976</v>
+        <v>-0.6192547717896785</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>2008</v>
       </c>
       <c r="B10">
         <v>551500</v>
       </c>
       <c r="C10">
-        <v>553764.562601121</v>
+        <v>553870.2957903675</v>
       </c>
       <c r="D10">
-        <v>-2264.562601121026</v>
+        <v>-2370.295790367527</v>
       </c>
       <c r="E10">
-        <v>-0.4089396025061647</v>
+        <v>-0.4279514190204293</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>2009</v>
       </c>
       <c r="B11">
         <v>557800</v>
       </c>
       <c r="C11">
-        <v>559041.9741951141</v>
+        <v>559156.9886639647</v>
       </c>
       <c r="D11">
-        <v>-1241.974195114104</v>
+        <v>-1356.988663964672</v>
       </c>
       <c r="E11">
-        <v>-0.2221611707962087</v>
+        <v>-0.2426847363934457</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>2010</v>
       </c>
       <c r="B12">
         <v>565300</v>
       </c>
       <c r="C12">
-        <v>565849.2196265807</v>
+        <v>565975.1799374919</v>
       </c>
       <c r="D12">
-        <v>-549.2196265807142</v>
+        <v>-675.1799374918919</v>
       </c>
       <c r="E12">
-        <v>-0.09706112645046311</v>
+        <v>-0.1192949728937691</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>2011</v>
       </c>
       <c r="B13">
         <v>564600</v>
       </c>
       <c r="C13">
-        <v>572792.1368948156</v>
+        <v>572932.6545736709</v>
       </c>
       <c r="D13">
-        <v>-8192.136894815601</v>
+        <v>-8332.654573670938</v>
       </c>
       <c r="E13">
-        <v>-1.430211130206203</v>
+        <v>-1.454386393785044</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>2012</v>
       </c>
       <c r="B14">
         <v>558500</v>
       </c>
       <c r="C14">
-        <v>578824.4175882342</v>
+        <v>578995.8276273068</v>
       </c>
       <c r="D14">
-        <v>-20324.41758823418</v>
+        <v>-20495.8276273068</v>
       </c>
       <c r="E14">
-        <v>-3.511326918950511</v>
+        <v>-3.539892111364185</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>2013</v>
       </c>
       <c r="B15">
         <v>560100</v>
       </c>
       <c r="C15">
-        <v>583982.5410920507</v>
+        <v>584190.1940168024</v>
       </c>
       <c r="D15">
-        <v>-23882.54109205073</v>
+        <v>-24090.19401680236</v>
       </c>
       <c r="E15">
-        <v>-4.089598474534912</v>
+        <v>-4.123690240529693</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>2014</v>
       </c>
       <c r="B16">
         <v>567300</v>
       </c>
       <c r="C16">
-        <v>591899.512944538</v>
+        <v>592115.0299842544</v>
       </c>
       <c r="D16">
-        <v>-24599.51294453803</v>
+        <v>-24815.02998425439</v>
       </c>
       <c r="E16">
-        <v>-4.156028583663161</v>
+        <v>-4.190913712309292</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>2015</v>
       </c>
       <c r="B17">
         <v>578900</v>
       </c>
       <c r="C17">
-        <v>603745.8957108234</v>
+        <v>603944.4211149375</v>
       </c>
       <c r="D17">
-        <v>-24845.89571082336</v>
+        <v>-25044.42111493752</v>
       </c>
       <c r="E17">
-        <v>-4.115290205256122</v>
+        <v>-4.14680891806289</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>2016</v>
       </c>
       <c r="B18">
         <v>594700</v>
       </c>
       <c r="C18">
-        <v>617107.0410197001</v>
+        <v>617287.0938656105</v>
       </c>
       <c r="D18">
-        <v>-22407.04101970012</v>
+        <v>-22587.09386561054</v>
       </c>
       <c r="E18">
-        <v>-3.630981260994041</v>
+        <v>-3.659090573911784</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>2017</v>
       </c>
       <c r="B19">
         <v>609200</v>
       </c>
       <c r="C19">
-        <v>631267.6762516528</v>
+        <v>631410.3692954445</v>
       </c>
       <c r="D19">
-        <v>-22067.67625165277</v>
+        <v>-22210.36929544446</v>
       </c>
       <c r="E19">
-        <v>-3.495771616675579</v>
+        <v>-3.517580701157595</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>2018</v>
       </c>
       <c r="B20">
         <v>619600</v>
       </c>
       <c r="C20">
-        <v>644104.3981900596</v>
+        <v>644192.5032100378</v>
       </c>
       <c r="D20">
-        <v>-24504.39819005958</v>
+        <v>-24592.50321003783</v>
       </c>
       <c r="E20">
-        <v>-3.804414045132623</v>
+        <v>-3.817570537920322</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>2019</v>
       </c>
       <c r="B21">
         <v>628200</v>
       </c>
       <c r="C21">
-        <v>655285.8842719045</v>
+        <v>655322.6097235683</v>
       </c>
       <c r="D21">
-        <v>-27085.88427190448</v>
+        <v>-27122.60972356831</v>
       </c>
       <c r="E21">
-        <v>-4.133445404825087</v>
+        <v>-4.138817938085383</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>2020</v>
       </c>
       <c r="B22">
         <v>639400</v>
       </c>
       <c r="C22">
-        <v>668026.9547377916</v>
+        <v>668009.5945787356</v>
       </c>
       <c r="D22">
-        <v>-28626.95473779156</v>
+        <v>-28609.59457873565</v>
       </c>
       <c r="E22">
-        <v>-4.285299348291713</v>
+        <v>-4.282811925295416</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>2021</v>
       </c>
       <c r="B23">
         <v>647400</v>
       </c>
       <c r="C23">
-        <v>673877.2248834948</v>
+        <v>673787.3964828703</v>
       </c>
       <c r="D23">
-        <v>-26477.22488349478</v>
+        <v>-26387.39648287033</v>
       </c>
       <c r="E23">
-        <v>-3.929087362771813</v>
+        <v>-3.91627932202516</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>2022</v>
       </c>
       <c r="B24">
         <v>652000</v>
       </c>
       <c r="C24">
-        <v>671878.8606435751</v>
+        <v>671726.9786689661</v>
       </c>
       <c r="D24">
-        <v>-19878.86064357508</v>
+        <v>-19726.9786689661</v>
       </c>
       <c r="E24">
-        <v>-2.958697141406361</v>
+        <v>-2.936755452052158</v>
       </c>
     </row>
   </sheetData>
@@ -1237,411 +1211,411 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>2000</v>
       </c>
       <c r="B2">
         <v>13129</v>
       </c>
       <c r="C2">
-        <v>13403.65890202668</v>
+        <v>13385.91504048598</v>
       </c>
       <c r="D2">
-        <v>-274.6589020266765</v>
+        <v>-256.9150404859811</v>
       </c>
       <c r="E2">
-        <v>-2.049133777830972</v>
+        <v>-1.919293822715415</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2001</v>
       </c>
       <c r="B3">
         <v>13794</v>
       </c>
       <c r="C3">
-        <v>13904.76554888965</v>
+        <v>13885.62249731768</v>
       </c>
       <c r="D3">
-        <v>-110.7655488896526</v>
+        <v>-91.62249731768316</v>
       </c>
       <c r="E3">
-        <v>-0.7966013414623708</v>
+        <v>-0.6598371613183498</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2002</v>
       </c>
       <c r="B4">
         <v>14800</v>
       </c>
       <c r="C4">
-        <v>14960.27863634488</v>
+        <v>14943.84358210379</v>
       </c>
       <c r="D4">
-        <v>-160.2786363448795</v>
+        <v>-143.8435821037929</v>
       </c>
       <c r="E4">
-        <v>-1.071361304431152</v>
+        <v>-0.9625608118386272</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>2003</v>
       </c>
       <c r="B5">
         <v>15794</v>
       </c>
       <c r="C5">
-        <v>16188.44070208509</v>
+        <v>16165.41077190083</v>
       </c>
       <c r="D5">
-        <v>-394.4407020850886</v>
+        <v>-371.4107719008316</v>
       </c>
       <c r="E5">
-        <v>-2.436557722537688</v>
+        <v>-2.297564702447451</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>2004</v>
       </c>
       <c r="B6">
         <v>17064</v>
       </c>
       <c r="C6">
-        <v>17448.55512474875</v>
+        <v>17421.60624530239</v>
       </c>
       <c r="D6">
-        <v>-384.5551247487456</v>
+        <v>-357.6062453023878</v>
       </c>
       <c r="E6">
-        <v>-2.203936784446403</v>
+        <v>-2.052659440623127</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>2005</v>
       </c>
       <c r="B7">
         <v>18671</v>
       </c>
       <c r="C7">
-        <v>18803.16292537983</v>
+        <v>18785.61193577181</v>
       </c>
       <c r="D7">
-        <v>-132.1629253798274</v>
+        <v>-114.6119357718089</v>
       </c>
       <c r="E7">
-        <v>-0.7028760315714684</v>
+        <v>-0.6101048832674084</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>2006</v>
       </c>
       <c r="B8">
         <v>19697</v>
       </c>
       <c r="C8">
-        <v>19735.89614215329</v>
+        <v>19720.63996221944</v>
       </c>
       <c r="D8">
-        <v>-38.89614215329129</v>
+        <v>-23.63996221944399</v>
       </c>
       <c r="E8">
-        <v>-0.1970832328723813</v>
+        <v>-0.1198742143497023</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>2007</v>
       </c>
       <c r="B9">
         <v>20981</v>
       </c>
       <c r="C9">
-        <v>20510.77778675365</v>
+        <v>20535.98000526109</v>
       </c>
       <c r="D9">
-        <v>470.2222132463467</v>
+        <v>445.0199947389119</v>
       </c>
       <c r="E9">
-        <v>2.292561589497729</v>
+        <v>2.167025847438996</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>2008</v>
       </c>
       <c r="B10">
         <v>22611</v>
       </c>
       <c r="C10">
-        <v>22038.62620168724</v>
+        <v>22058.13548824816</v>
       </c>
       <c r="D10">
-        <v>572.3737983127612</v>
+        <v>552.864511751839</v>
       </c>
       <c r="E10">
-        <v>2.597139191321014</v>
+        <v>2.506397297479594</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>2009</v>
       </c>
       <c r="B11">
         <v>23342</v>
       </c>
       <c r="C11">
-        <v>21853.26378197067</v>
+        <v>21903.10623419921</v>
       </c>
       <c r="D11">
-        <v>1488.736218029328</v>
+        <v>1438.893765800793</v>
       </c>
       <c r="E11">
-        <v>6.812420482736135</v>
+        <v>6.569359388642894</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>2010</v>
       </c>
       <c r="B12">
         <v>23980</v>
       </c>
       <c r="C12">
-        <v>22619.31206616836</v>
+        <v>22622.32181288475</v>
       </c>
       <c r="D12">
-        <v>1360.687933831636</v>
+        <v>1357.678187115253</v>
       </c>
       <c r="E12">
-        <v>6.015602640129859</v>
+        <v>6.001497982147768</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>2011</v>
       </c>
       <c r="B13">
         <v>25194</v>
       </c>
       <c r="C13">
-        <v>23663.38964893337</v>
+        <v>23664.38036372572</v>
       </c>
       <c r="D13">
-        <v>1530.610351066625</v>
+        <v>1529.619636274278</v>
       </c>
       <c r="E13">
-        <v>6.468263312122816</v>
+        <v>6.463805993496353</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>2012</v>
       </c>
       <c r="B14">
         <v>26537</v>
       </c>
       <c r="C14">
-        <v>24852.6007678224</v>
+        <v>24867.33212940194</v>
       </c>
       <c r="D14">
-        <v>1684.399232177602</v>
+        <v>1669.667870598063</v>
       </c>
       <c r="E14">
-        <v>6.777557197790171</v>
+        <v>6.714302370313091</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>2013</v>
       </c>
       <c r="B15">
         <v>27715</v>
       </c>
       <c r="C15">
-        <v>25617.27321618682</v>
+        <v>25634.10556249695</v>
       </c>
       <c r="D15">
-        <v>2097.726783813177</v>
+        <v>2080.894437503051</v>
       </c>
       <c r="E15">
-        <v>8.188720033198866</v>
+        <v>8.117679130366962</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>2014</v>
       </c>
       <c r="B16">
         <v>30735</v>
       </c>
       <c r="C16">
-        <v>27079.19176438572</v>
+        <v>27101.50915744621</v>
       </c>
       <c r="D16">
-        <v>3655.808235614277</v>
+        <v>3633.490842553794</v>
       </c>
       <c r="E16">
-        <v>13.50043334905718</v>
+        <v>13.40696867264856</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>2015</v>
       </c>
       <c r="B17">
         <v>32106</v>
       </c>
       <c r="C17">
-        <v>28876.09019183733</v>
+        <v>28924.90985626361</v>
       </c>
       <c r="D17">
-        <v>3229.909808162669</v>
+        <v>3181.090143736386</v>
       </c>
       <c r="E17">
-        <v>11.18541252193379</v>
+        <v>10.99775300785433</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>2016</v>
       </c>
       <c r="B18">
         <v>33132</v>
       </c>
       <c r="C18">
-        <v>31280.81760301127</v>
+        <v>31367.33230213309</v>
       </c>
       <c r="D18">
-        <v>1851.18239698873</v>
+        <v>1764.667697866913</v>
       </c>
       <c r="E18">
-        <v>5.917947607643493</v>
+        <v>5.625813763406681</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>2017</v>
       </c>
       <c r="B19">
         <v>34156</v>
       </c>
       <c r="C19">
-        <v>33403.55688457763</v>
+        <v>33515.44365851385</v>
       </c>
       <c r="D19">
-        <v>752.4431154223712</v>
+        <v>640.5563414861463</v>
       </c>
       <c r="E19">
-        <v>2.252583813221918</v>
+        <v>1.911227397174637</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>2018</v>
       </c>
       <c r="B20">
         <v>36689</v>
       </c>
       <c r="C20">
-        <v>35649.59629463434</v>
+        <v>35750.83377560642</v>
       </c>
       <c r="D20">
-        <v>1039.403705365665</v>
+        <v>938.1662243935789</v>
       </c>
       <c r="E20">
-        <v>2.915611432946596</v>
+        <v>2.624179984953834</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>2019</v>
       </c>
       <c r="B21">
         <v>38297</v>
       </c>
       <c r="C21">
-        <v>37670.60843130637</v>
+        <v>37747.53732496355</v>
       </c>
       <c r="D21">
-        <v>626.3915686936307</v>
+        <v>549.4626750364478</v>
       </c>
       <c r="E21">
-        <v>1.662812454531699</v>
+        <v>1.455625224782736</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>2020</v>
       </c>
       <c r="B22">
         <v>40525</v>
       </c>
       <c r="C22">
-        <v>39505.06178034595</v>
+        <v>39609.98242851395</v>
       </c>
       <c r="D22">
-        <v>1019.938219654046</v>
+        <v>915.0175714860525</v>
       </c>
       <c r="E22">
-        <v>2.581791227982519</v>
+        <v>2.310068107546952</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>2021</v>
       </c>
       <c r="B23">
         <v>40267</v>
       </c>
       <c r="C23">
-        <v>40464.66284321398</v>
+        <v>40481.51672776663</v>
       </c>
       <c r="D23">
-        <v>-197.6628432139769</v>
+        <v>-214.5167277666333</v>
       </c>
       <c r="E23">
-        <v>-0.4884826150160928</v>
+        <v>-0.5299127728074832</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>2022</v>
       </c>
       <c r="B24">
         <v>43981</v>
       </c>
       <c r="C24">
-        <v>44347.6215755955</v>
+        <v>44395.46659297859</v>
       </c>
       <c r="D24">
-        <v>-366.6215755954981</v>
+        <v>-414.4665929785915</v>
       </c>
       <c r="E24">
-        <v>-0.8266995220263402</v>
+        <v>-0.9335786394103174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>